<commit_message>
feat: new master sheet layout etc.
</commit_message>
<xml_diff>
--- a/data/excel_dumps/students/ikleiman@stonybrook.edu.xlsx
+++ b/data/excel_dumps/students/ikleiman@stonybrook.edu.xlsx
@@ -26,6 +26,9 @@
     <t>Correct</t>
   </si>
   <si>
+    <t>Elapsed Time</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -33,9 +36,6 @@
   </si>
   <si>
     <t>2019-10-21</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -382,7 +382,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,75 +395,178 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>